<commit_message>
Add importance ranking and shap by postcode for distance scripts
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/dist_LR/Berlin.xlsx
+++ b/outputs/ML_Results/dist_LR/Berlin.xlsx
@@ -7,56 +7,56 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ27771009" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ27890794" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="summ28000145" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ28115658" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ28242873" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ28372391" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="summ28502907" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ28634314" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="summ28772307" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="summ28906468" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="summ29041513" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="summ29175776" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="summ29307801" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="summ29445203" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="summ29579935" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="summ29714444" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="summ29849918" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="summ29985427" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="summ30118942" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="summ30254306" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="summ30389895" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="summ30523247" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="summ30656282" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="summ30789820" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="summ30923097" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="summ31055131" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="summ31186834" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="summ31324358" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="summ31458072" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="summ31591587" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="summ31721421" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="summ31856466" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="summ31992814" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="summ32124334" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="summ32259371" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="summ32388878" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="summ32519390" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="summ32654427" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="summ32790937" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="summ32922448" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="summ33056716" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="summ33191233" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="summ33324272" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="summ33458636" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="summ33590151" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="summ33726200" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="summ33862958" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet name="summ34034485" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet name="summ34168515" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet name="summ34300031" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="summ01319359" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ01443819" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ01569287" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="summ01681272" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ01790130" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ01902538" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ02014848" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="summ02118752" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ02232015" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="summ02343920" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="summ02452467" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="summ02568254" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="summ02675354" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="summ02789293" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="summ02900874" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="summ03011783" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="summ03128970" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="summ03261968" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="summ03415455" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="summ03574817" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="summ03725965" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="summ03920943" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="summ04098836" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="summ04278905" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="summ04453445" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="summ04641131" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="summ04829886" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="summ05004498" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="summ05154973" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="summ05309897" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="summ05457771" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="summ05604116" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="summ05786958" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="summ05968031" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="summ06129371" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="summ06279101" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="summ06441137" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="summ06615117" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="summ06776367" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="summ06927420" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="summ07133643" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="summ07292148" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="summ07449600" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="summ07601347" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="summ07763778" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="summ07945161" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="summ08108533" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="summ08258140" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="summ08421051" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="summ08578059" sheetId="50" state="visible" r:id="rId50"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
rerun LU d2c FeatEng for FR cities with new spatial units, and dist models
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/dist_LR/Berlin.xlsx
+++ b/outputs/ML_Results/dist_LR/Berlin.xlsx
@@ -7,56 +7,56 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ16803226" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ16929936" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="summ17065237" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ17180605" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ17314453" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ17465544" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="summ17662450" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ17794640" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="summ17928970" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="summ18063682" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="summ18213982" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="summ18346821" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="summ18483170" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="summ18630046" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="summ18783004" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="summ18930924" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="summ19063606" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="summ19214194" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="summ19329927" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="summ19463402" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="summ19597512" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="summ19729805" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="summ19861265" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="summ19997495" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="summ20130050" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="summ20263392" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="summ20397804" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="summ20530080" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="summ20663406" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="summ20796859" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="summ20929614" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="summ21064766" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="summ21207222" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="summ21352050" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="summ21480847" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="summ21612305" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="summ21761226" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="summ21879511" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="summ22029943" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="summ22163891" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="summ22311236" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="summ22430386" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="summ22563639" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="summ22697024" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="summ22828913" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="summ22947099" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="summ23080018" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet name="summ23208687" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet name="summ23353535" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet name="summ23480159" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="summ49401962" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ49520588" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ49622465" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="summ49725367" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ49822326" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ49923252" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ50022188" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="summ50123029" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ50225579" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="summ50389253" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="summ50500292" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="summ50610560" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="summ50718558" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="summ50827392" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="summ50930329" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="summ51022285" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="summ51132405" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="summ51222819" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="summ51323062" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="summ51423363" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="summ51522815" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="summ51623435" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="summ51722850" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="summ51822947" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="summ51928940" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="summ52022608" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="summ52122925" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="summ52227908" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="summ52326247" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="summ52422732" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="summ52521433" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="summ52624906" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="summ52721405" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="summ52822337" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="summ52924446" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="summ53033892" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="summ53131561" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="summ53228943" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="summ53340787" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="summ53440607" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="summ53547872" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="summ53639103" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="summ53744713" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="summ53853899" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="summ53957683" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="summ54055873" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="summ54164321" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="summ54257928" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="summ54360641" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="summ54464956" sheetId="50" state="visible" r:id="rId50"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>